<commit_message>
[Saurav] New User Created
</commit_message>
<xml_diff>
--- a/TestData/OpenHRM.xlsx
+++ b/TestData/OpenHRM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse\Opensource-OrangeHRM\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CD0924-BD2D-47EE-BBC4-0C16D95D66E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A056CD-0A43-48C3-BC1C-17A0019C5C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05A06626-5E96-4550-8DA5-D0486DC003AA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Dashboard</t>
   </si>
@@ -85,9 +85,6 @@
     <t xml:space="preserve">Employee Name </t>
   </si>
   <si>
-    <t>Peter Mac Anderson</t>
-  </si>
-  <si>
     <t>Status Label</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>Save button</t>
   </si>
   <si>
-    <t xml:space="preserve">Save </t>
-  </si>
-  <si>
     <t xml:space="preserve">UserName </t>
   </si>
   <si>
@@ -131,6 +125,27 @@
   </si>
   <si>
     <t>Ryukas</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Select Role</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>Seletc status</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Lisa Michelle Walker</t>
   </si>
 </sst>
 </file>
@@ -493,9 +508,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE950849-8C7D-4F32-85F2-0BD9E98D9F27}">
-  <dimension ref="A2:B18"/>
+  <dimension ref="A2:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -573,72 +588,94 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Saurav] : Open Source - Orange HRM
</commit_message>
<xml_diff>
--- a/TestData/OpenHRM.xlsx
+++ b/TestData/OpenHRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse\Opensource-OrangeHRM\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311D7126-6FE6-44F9-BB74-6C7CDC8F13DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1150F48-BC25-44F3-927E-0925FE54AE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05A06626-5E96-4550-8DA5-D0486DC003AA}"/>
+    <workbookView xWindow="4530" yWindow="2520" windowWidth="15375" windowHeight="7875" xr2:uid="{05A06626-5E96-4550-8DA5-D0486DC003AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Dashboard</t>
   </si>
@@ -56,9 +56,6 @@
 User Management</t>
   </si>
   <si>
-    <t xml:space="preserve">Add </t>
-  </si>
-  <si>
     <t>Add button</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>Password&amp;1234</t>
   </si>
   <si>
-    <t>Ryukas</t>
-  </si>
-  <si>
     <t>Save</t>
   </si>
   <si>
@@ -173,7 +167,25 @@
     <t>s</t>
   </si>
   <si>
-    <t>Charlie  Carter</t>
+    <t>Success Message</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>naveen  a</t>
+  </si>
+  <si>
+    <t>aurasd312</t>
   </si>
 </sst>
 </file>
@@ -536,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE950849-8C7D-4F32-85F2-0BD9E98D9F27}">
-  <dimension ref="A2:C20"/>
+  <dimension ref="A2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +560,7 @@
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -556,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -564,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -572,138 +584,155 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -730,62 +759,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>